<commit_message>
Added Visuals and moved some data
</commit_message>
<xml_diff>
--- a/Data/Study Responses.xlsx
+++ b/Data/Study Responses.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="68" documentId="8_{A2B540A0-4E65-454A-A625-C921F2F1A0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18E392CD-82F8-47F5-92D8-9AB9D828541A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{57E2499E-635E-4473-A2EA-1DDCD5DFEE34}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{57E2499E-635E-4473-A2EA-1DDCD5DFEE34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,16 +486,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE4BF9C-BD83-4AC3-8085-66E7E77F57D7}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="47.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -511,7 +511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -519,7 +519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -527,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -543,7 +543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -551,7 +551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -559,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -567,7 +567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -575,7 +575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -583,7 +583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -591,7 +591,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -599,7 +599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -607,7 +607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -615,7 +615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -623,7 +623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -631,7 +631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -639,7 +639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -647,7 +647,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -655,7 +655,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5</v>
       </c>
@@ -663,7 +663,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -671,7 +671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -679,7 +679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -687,7 +687,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -695,7 +695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -703,7 +703,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -711,7 +711,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -719,7 +719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -727,7 +727,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>

</xml_diff>